<commit_message>
it is working until line 40 on main api
</commit_message>
<xml_diff>
--- a/transfer.xlsx
+++ b/transfer.xlsx
@@ -2,9 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9660" windowWidth="16095" xWindow="240" yWindow="15"/>
   </bookViews>
   <sheets>
     <sheet name="abdallah" sheetId="1" state="visible" r:id="rId1"/>
@@ -24,10 +23,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
@@ -44,12 +51,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -60,18 +82,21 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="3">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -434,7 +459,7 @@
   </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -473,7 +498,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
@@ -492,39 +517,39 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>מקט</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>מספר הזמנה</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>סוג</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>אזור_במחסן</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>מיקום</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>משטח</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -543,39 +568,39 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>מקט</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>מספר הזמנה</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>סוג</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>אזור_במחסן</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>מיקום</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>משטח</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -594,39 +619,39 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>מקט</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>מספר הזמנה</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>סוג</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>אזור_במחסן</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>מיקום</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>משטח</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -645,39 +670,39 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>מקט</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>מספר הזמנה</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>סוג</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>אזור_במחסן</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>מיקום</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>משטח</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -696,39 +721,39 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>מקט</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>מספר הזמנה</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>סוג</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>אזור_במחסן</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>מיקום</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>משטח</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -747,32 +772,32 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>מקט</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>מספר הזמנה</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>סוג</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>אזור_במחסן</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>מיקום</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>משטח</t>
         </is>
@@ -843,7 +868,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -862,32 +887,32 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>מקט</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>מספר הזמנה</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>סוג</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>אזור_במחסן</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>מיקום</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>משטח</t>
         </is>
@@ -958,6 +983,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>